<commit_message>
Updated Cesarini sample size
</commit_message>
<xml_diff>
--- a/adoptive_sibling_correlations.xlsx
+++ b/adoptive_sibling_correlations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srivinay Tummarakota\Documents\VinaysDocs\Unboxing Politics\Missing Heritability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srivinay Tummarakota\Documents\VinaysDocs\Unboxing Politics\Missing Heritability\missing-heritability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022DB711-499B-4E10-B725-4EF9DAB8C1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9C9B32-6E17-433C-9826-B40BC9ACF820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>study</t>
   </si>
@@ -129,27 +129,6 @@
   </si>
   <si>
     <t>Sample size is listed in https://www.nature.com/articles/s41539-017-0005-6</t>
-  </si>
-  <si>
-    <t>Sample size sh listed al https://www.nature.com/articles/s41539-002-0005-2</t>
-  </si>
-  <si>
-    <t>Sample size ev listed  a https://www.nature.com/articles/s41539-003-0005-8</t>
-  </si>
-  <si>
-    <t>Sample size ev listed  e https://www.nature.com/articles/s41539-0192-0005-1</t>
-  </si>
-  <si>
-    <t>Sample size -R listed in https://www.nature.com/articles/s41539-009-0005-7</t>
-  </si>
-  <si>
-    <t>Sample size -R listed in https://www.nature.com/articles/s41539-005-0005-1</t>
-  </si>
-  <si>
-    <t>Sample size se listed in https://www.nature.com/articles/s41539-002-0005-7</t>
-  </si>
-  <si>
-    <t>Sample size se listed in https://www.nature.com/articles/s41539-003-0005-1</t>
   </si>
 </sst>
 </file>
@@ -470,7 +449,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>